<commit_message>
Updated Meetings Logs up to 12/2/18
</commit_message>
<xml_diff>
--- a/docs/gantt_meeting-logs/Meeting Logs.xlsx
+++ b/docs/gantt_meeting-logs/Meeting Logs.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="26915"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21029"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Zach/Repos/BitsPlease-FESP/docs/gantt/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Gager\Documents\GitHub\BitsPlease-FESP\docs\gantt_meeting-logs\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DC214577-CCE5-4CF9-B788-E978E770CF80}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="640" yWindow="1180" windowWidth="28160" windowHeight="16880" tabRatio="500"/>
+    <workbookView xWindow="645" yWindow="1185" windowWidth="28155" windowHeight="16875" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Meeting Logs" sheetId="2" r:id="rId1"/>
@@ -35,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="41">
   <si>
     <t>Date</t>
   </si>
@@ -146,15 +147,37 @@
   </si>
   <si>
     <t>Finished documentation, wrote tests, tied up loose ends</t>
+  </si>
+  <si>
+    <t>Worked out artifacts and documentation that still needed to be done, set up another meeting to work on these</t>
+  </si>
+  <si>
+    <t>Gage, Jacob, Zach</t>
+  </si>
+  <si>
+    <t>Working on remaining artifacts and documentation</t>
+  </si>
+  <si>
+    <t>Spahr Library</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="m/d/yy"/>
+  </numFmts>
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -194,32 +217,37 @@
   </borders>
   <cellStyleXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
-    <xf numFmtId="14" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
+    <xf numFmtId="14" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
-    <xf numFmtId="14" fontId="1" fillId="0" borderId="0" xfId="1" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="14" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="4">
-    <cellStyle name="Date" xfId="2"/>
+    <cellStyle name="Date" xfId="2" xr:uid="{00000000-0005-0000-0000-000000000000}"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal 2" xfId="1"/>
-    <cellStyle name="zHiddenText" xfId="3"/>
+    <cellStyle name="Normal 2" xfId="1" xr:uid="{00000000-0005-0000-0000-000002000000}"/>
+    <cellStyle name="zHiddenText" xfId="3" xr:uid="{00000000-0005-0000-0000-000003000000}"/>
   </cellStyles>
   <dxfs count="5">
     <dxf>
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" justifyLastLine="0" shrinkToFit="0"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="19" formatCode="m/d/yy"/>
+      <numFmt numFmtId="164" formatCode="m/d/yy"/>
     </dxf>
     <dxf>
       <fill>
@@ -272,7 +300,7 @@
     </dxf>
   </dxfs>
   <tableStyles count="1" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium7">
-    <tableStyle name="Gantt Table Style" pivot="0" count="3">
+    <tableStyle name="Gantt Table Style" pivot="0" count="3" xr9:uid="{00000000-0011-0000-FFFF-FFFF00000000}">
       <tableStyleElement type="wholeTable" dxfId="4"/>
       <tableStyleElement type="headerRow" dxfId="3"/>
       <tableStyleElement type="firstRowStripe" dxfId="2"/>
@@ -281,6 +309,9 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -291,37 +322,22 @@
   <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
     <sheetNames>
       <sheetName val="Gantt"/>
-      <sheetName val="Meeting Logs"/>
-      <sheetName val="About"/>
     </sheetNames>
     <sheetDataSet>
-      <sheetData sheetId="0">
-        <row r="3">
-          <cell r="F3">
-            <v>43378</v>
-          </cell>
-        </row>
-        <row r="4">
-          <cell r="F4">
-            <v>0</v>
-          </cell>
-        </row>
-      </sheetData>
-      <sheetData sheetId="1"/>
-      <sheetData sheetId="2"/>
+      <sheetData sheetId="0" refreshError="1"/>
     </sheetDataSet>
   </externalBook>
 </externalLink>
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table2" displayName="Table2" ref="A1:D25" totalsRowShown="0">
-  <autoFilter ref="A1:D25"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table2" displayName="Table2" ref="A1:D26" totalsRowShown="0">
+  <autoFilter ref="A1:D26" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
   <tableColumns count="4">
-    <tableColumn id="1" name="Date" dataDxfId="1"/>
-    <tableColumn id="2" name="Location"/>
-    <tableColumn id="3" name="Members"/>
-    <tableColumn id="4" name="Things Discussed" dataDxfId="0"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Date" dataDxfId="1"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Location"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Members"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="Things Discussed" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="Gantt Table Style" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -589,21 +605,23 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D25"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:D26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A15" sqref="A15"/>
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="17" defaultRowHeight="23" customHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="17" defaultRowHeight="23.1" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="3" width="17" style="1"/>
-    <col min="4" max="4" width="50.5" style="1" customWidth="1"/>
+    <col min="1" max="1" width="9.375" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.875" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.875" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="50.25" style="1" bestFit="1" customWidth="1"/>
     <col min="5" max="16384" width="17" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="23" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -617,7 +635,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="30" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A2" s="2">
         <v>43378</v>
       </c>
@@ -631,7 +649,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="30" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A3" s="2">
         <v>43383</v>
       </c>
@@ -645,7 +663,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="23" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A4" s="2">
         <v>43385</v>
       </c>
@@ -659,7 +677,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="5" spans="1:4" ht="30" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A5" s="2">
         <v>43388</v>
       </c>
@@ -673,7 +691,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="6" spans="1:4" ht="30" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A6" s="2">
         <v>43389</v>
       </c>
@@ -687,7 +705,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="7" spans="1:4" ht="30" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A7" s="2">
         <v>43390</v>
       </c>
@@ -701,7 +719,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="8" spans="1:4" ht="30" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A8" s="2">
         <v>43392</v>
       </c>
@@ -715,7 +733,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="9" spans="1:4" ht="23" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A9" s="2">
         <v>43397</v>
       </c>
@@ -729,7 +747,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="10" spans="1:4" ht="23" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A10" s="2">
         <v>43399</v>
       </c>
@@ -743,7 +761,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="11" spans="1:4" ht="23" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A11" s="2">
         <v>43402</v>
       </c>
@@ -757,7 +775,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="12" spans="1:4" ht="23" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A12" s="2">
         <v>43404</v>
       </c>
@@ -768,21 +786,21 @@
         <v>20</v>
       </c>
     </row>
-    <row r="13" spans="1:4" ht="23" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A13" s="2">
         <v>43407</v>
       </c>
       <c r="B13" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="C13" s="1" t="s">
+      <c r="C13" s="3" t="s">
         <v>21</v>
       </c>
       <c r="D13" s="3" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="14" spans="1:4" ht="23" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A14" s="2">
         <v>43411</v>
       </c>
@@ -796,7 +814,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="15" spans="1:4" ht="23" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="A15" s="2">
         <v>43413</v>
       </c>
@@ -810,7 +828,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="16" spans="1:4" ht="30" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A16" s="2">
         <v>43414</v>
       </c>
@@ -824,7 +842,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="17" spans="1:4" ht="23" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A17" s="2">
         <v>43416</v>
       </c>
@@ -838,7 +856,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="18" spans="1:4" ht="30" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A18" s="2">
         <v>43417</v>
       </c>
@@ -852,7 +870,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="19" spans="1:4" ht="23" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A19" s="2">
         <v>43418</v>
       </c>
@@ -866,7 +884,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="20" spans="1:4" ht="23" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A20" s="2">
         <v>43420</v>
       </c>
@@ -880,7 +898,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="21" spans="1:4" ht="23" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A21" s="2">
         <v>43423</v>
       </c>
@@ -894,7 +912,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="22" spans="1:4" ht="23" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A22" s="2">
         <v>43427</v>
       </c>
@@ -908,7 +926,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="23" spans="1:4" ht="23" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A23" s="2">
         <v>43428</v>
       </c>
@@ -922,7 +940,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="24" spans="1:4" ht="23" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A24" s="2">
         <v>43429</v>
       </c>
@@ -936,26 +954,50 @@
         <v>36</v>
       </c>
     </row>
-    <row r="25" spans="1:4" ht="23" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A25" s="2"/>
-      <c r="D25" s="3"/>
+    <row r="25" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A25" s="2">
+        <v>43434</v>
+      </c>
+      <c r="B25" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="C25" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="D25" s="6" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A26" s="5">
+        <v>43436</v>
+      </c>
+      <c r="B26" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="C26" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="D26" s="6" t="s">
+        <v>39</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
   <tableParts count="1">
-    <tablePart r:id="rId1"/>
+    <tablePart r:id="rId2"/>
   </tableParts>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>